<commit_message>
Remove light chain unknown from xlsx files
</commit_message>
<xml_diff>
--- a/examples/antibodies-submission.xlsx
+++ b/examples/antibodies-submission.xlsx
@@ -488,7 +488,7 @@
       <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve">- Affinity: Spike protein binding affinity; inhibition of ACE2 binding; ELISA for Spike </t>
+          <t>- Affinity: Spike protein binding affinity; inhibition of ACE2 binding; ELISA for Spike</t>
         </is>
       </c>
     </row>
@@ -639,7 +639,7 @@
       <formula1>=Terminology!$B$2:$B$15</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="D2:D100" type="list">
-      <formula1>=Terminology!$C$2:$C$4</formula1>
+      <formula1>=Terminology!$C$2:$C$3</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="E2:E100" type="list">
       <formula1>=Terminology!$D$2:$D$12</formula1>
@@ -747,11 +747,7 @@
           <t>IgA2</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
           <t>IGHV2-5</t>

</xml_diff>